<commit_message>
Added ExcelReader (not working yet), created AddCustomerTest
</commit_message>
<xml_diff>
--- a/SeleniumTestFramework/src/test/resources/excel/testdata.xlsx
+++ b/SeleniumTestFramework/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\SeleniumTestFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA45373B-9A2A-44D8-B159-4A637B5E872F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730FB73B-B221-41C0-AF36-C5EC1E6CAD1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6F378EB-DA98-4D33-AC4B-9EC1803C6080}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,6 +27,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Raman</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t>A234wd</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,12 +400,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F7C610-ADBA-4227-BE2C-82ED89188EF8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>